<commit_message>
Remove time from imports
</commit_message>
<xml_diff>
--- a/server/logs.xlsx
+++ b/server/logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_4F599E0CC6D4DD4A53D7C1704716687674D97B51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14F010EA-1A16-4690-8DF4-81016375D328}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_4F599E0CC6145D25085813A1723373294D7F7363" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21E37C5-4A7D-4A96-8BE6-BFAA6FC89290}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>